<commit_message>
Ajout d'un fichier excel de test
</commit_message>
<xml_diff>
--- a/liste des test.xlsx
+++ b/liste des test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seemt\Desktop\HEIG-VD\Semestre3\POO\Labo\Labo8\Labo8\POO-Labo_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23978FD0-8501-4FC3-815E-DBFE938F37FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528E4A0D-35BF-475C-A76A-BC1352835018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{477B09BC-C81F-481D-B86E-8C2C2F190558}"/>
   </bookViews>
@@ -33,6 +33,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Test déplacement pion</t>
+  </si>
+  <si>
+    <t>Avancer un pion de 1</t>
+  </si>
+  <si>
+    <t>Avancer un pion de 2 au premier coup</t>
+  </si>
+  <si>
+    <t>Avancer un pion de 1 puit de 2</t>
+  </si>
+  <si>
+    <t>Action effectuée</t>
+  </si>
+  <si>
+    <t>Résultat attendu</t>
+  </si>
+  <si>
+    <t>Résultat obtenu</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -44,15 +70,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,12 +92,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +429,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D944D000-6100-4BF9-8EA9-1B2AEDF837AE}">
-  <dimension ref="A1"/>
+  <dimension ref="D6:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="30.734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.62890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1015625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>